<commit_message>
Codigos Finales y Ajustes Finales
</commit_message>
<xml_diff>
--- a/Labs/Codigos_benchmark/Benchmark gráficas.xlsx
+++ b/Labs/Codigos_benchmark/Benchmark gráficas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvggt-my.sharepoint.com/personal/gar19085_uvg_edu_gt/Documents/UVG/Tesis/Tesis_Rodrigo_Garcia/Labs/Codigos_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="81" documentId="8_{FABDD7FD-6743-4204-B2FA-80C56CAF88A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3AFB86C6-4CE0-4491-B4E9-AA616B2182E3}"/>
+  <xr:revisionPtr revIDLastSave="107" documentId="8_{FABDD7FD-6743-4204-B2FA-80C56CAF88A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2382005F-8A69-45A1-92BE-7CC5B1BDB98C}"/>
   <bookViews>
-    <workbookView xWindow="-14400" yWindow="15" windowWidth="14400" windowHeight="15750" xr2:uid="{02B580AD-A341-4B04-B4A3-94A7FA17B0AB}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{02B580AD-A341-4B04-B4A3-94A7FA17B0AB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -833,6 +833,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -895,10 +948,71 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t> de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="low"/>
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="rnd">
@@ -1748,6 +1862,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1810,6 +1983,70 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="2.5000000000000001E-2"/>
+              <c:y val="0.343267351997667"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2359,6 +2596,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="dk1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="dk1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2421,6 +2717,59 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:sysClr val="windowText" lastClr="000000"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2607,26 +2956,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -2970,6 +3299,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3032,6 +3383,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3218,26 +3591,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -3581,6 +3934,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3643,6 +4018,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3829,26 +4226,6 @@
         </a:ln>
         <a:effectLst/>
       </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="20" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="dk1">
-                  <a:lumMod val="50000"/>
-                  <a:lumOff val="50000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -4192,6 +4569,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>No. de Intentos</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4254,6 +4653,28 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000"/>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Porcentaje de CPU</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="0.000" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -4512,126 +4933,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
   <cs:axisTitle>
@@ -5735,1659 +6036,6 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2"/>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:alpha val="70000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="2">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="1"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:shade val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="75000"/>
-          <a:lumOff val="25000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:legend>
-  <cs:plotArea>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:gradFill>
-        <a:gsLst>
-          <a:gs pos="100000">
-            <a:schemeClr val="lt1">
-              <a:lumMod val="95000"/>
-            </a:schemeClr>
-          </a:gs>
-          <a:gs pos="0">
-            <a:schemeClr val="lt1">
-              <a:alpha val="0"/>
-            </a:schemeClr>
-          </a:gs>
-        </a:gsLst>
-        <a:lin ang="5400000" scaled="0"/>
-      </a:gradFill>
-    </cs:spPr>
-  </cs:plotArea>
-  <cs:plotArea3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="20000"/>
-            <a:lumOff val="80000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="50000"/>
-        <a:lumOff val="50000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" kern="1200" cap="none" spc="20" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200" spc="0" baseline="0"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="246">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -8157,6 +6805,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8459,7 +7111,7 @@
   <dimension ref="A1:S44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="P40" sqref="P40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>